<commit_message>
fix data on emission bc deleted on Dbnomics
</commit_message>
<xml_diff>
--- a/Utils/myobs.xlsx
+++ b/Utils/myobs.xlsx
@@ -13,7 +13,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <t>eff_sample</t>
+  </si>
+  <si>
+    <t>gy_obs</t>
+  </si>
+  <si>
+    <t>gc_obs</t>
+  </si>
+  <si>
+    <t>gi_obs</t>
+  </si>
+  <si>
+    <t>pi_obs</t>
+  </si>
+  <si>
+    <t>r_obs</t>
+  </si>
+  <si>
+    <t>l_obs</t>
+  </si>
+  <si>
+    <t>co2_obs</t>
+  </si>
   <si>
     <t>eff_sample</t>
   </si>
@@ -97,28 +121,28 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
estimate with emissions + make all policy codes run
</commit_message>
<xml_diff>
--- a/Utils/myobs.xlsx
+++ b/Utils/myobs.xlsx
@@ -13,7 +13,55 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
+  <si>
+    <t>eff_sample</t>
+  </si>
+  <si>
+    <t>gy_obs</t>
+  </si>
+  <si>
+    <t>gc_obs</t>
+  </si>
+  <si>
+    <t>gi_obs</t>
+  </si>
+  <si>
+    <t>pi_obs</t>
+  </si>
+  <si>
+    <t>r_obs</t>
+  </si>
+  <si>
+    <t>l_obs</t>
+  </si>
+  <si>
+    <t>co2_obs</t>
+  </si>
+  <si>
+    <t>eff_sample</t>
+  </si>
+  <si>
+    <t>gy_obs</t>
+  </si>
+  <si>
+    <t>gc_obs</t>
+  </si>
+  <si>
+    <t>gi_obs</t>
+  </si>
+  <si>
+    <t>pi_obs</t>
+  </si>
+  <si>
+    <t>r_obs</t>
+  </si>
+  <si>
+    <t>l_obs</t>
+  </si>
+  <si>
+    <t>co2_obs</t>
+  </si>
   <si>
     <t>eff_sample</t>
   </si>
@@ -241,28 +289,28 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
addpath Data + read me toolbox requirements
</commit_message>
<xml_diff>
--- a/Utils/myobs.xlsx
+++ b/Utils/myobs.xlsx
@@ -13,7 +13,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
+  <si>
+    <t>eff_sample</t>
+  </si>
+  <si>
+    <t>gy_obs</t>
+  </si>
+  <si>
+    <t>gc_obs</t>
+  </si>
+  <si>
+    <t>gi_obs</t>
+  </si>
+  <si>
+    <t>pi_obs</t>
+  </si>
+  <si>
+    <t>r_obs</t>
+  </si>
+  <si>
+    <t>l_obs</t>
+  </si>
+  <si>
+    <t>co2_obs</t>
+  </si>
   <si>
     <t>eff_sample</t>
   </si>
@@ -289,28 +313,28 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2">

</xml_diff>